<commit_message>
feat: comp-organ lab3 submit version
</commit_message>
<xml_diff>
--- a/comp-organ/lab3/booth2/debug-booth2.xlsx
+++ b/comp-organ/lab3/booth2/debug-booth2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\computer-system\comp-organ\lab3\booth2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA6788-3E5C-42DB-85D1-86CCF95A6F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573988BC-57EA-46E1-B850-B47D7907D76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>-x补码</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +76,10 @@
   </si>
   <si>
     <t>yn+2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -209,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -334,11 +338,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -523,9 +611,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -564,20 +649,54 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -860,45 +979,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY42"/>
+  <dimension ref="A1:AZ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S1" sqref="D1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="3.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="3.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="3.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="3.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="2.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="2.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="2.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="2.6640625" style="82" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="2.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="2.5546875" style="78" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="2.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="2.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="44" max="47" width="2.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="48" max="51" width="2.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="3.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="3.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="3.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="3.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="2.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="2.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="2.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.6640625" style="81" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="2.5546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="2.5546875" style="77" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="2.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="44" width="2.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="45" max="48" width="2.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="52" width="2.5546875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10">
-        <v>0</v>
-      </c>
-      <c r="D1" s="11">
+      <c r="D1" s="10">
         <v>0</v>
       </c>
       <c r="E1" s="11">
@@ -907,7 +1024,7 @@
       <c r="F1" s="11">
         <v>0</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="11">
         <v>0</v>
       </c>
       <c r="H1" s="12">
@@ -916,10 +1033,10 @@
       <c r="I1" s="12">
         <v>0</v>
       </c>
-      <c r="J1" s="13">
-        <v>0</v>
-      </c>
-      <c r="K1" s="11">
+      <c r="J1" s="12">
+        <v>0</v>
+      </c>
+      <c r="K1" s="13">
         <v>0</v>
       </c>
       <c r="L1" s="11">
@@ -931,27 +1048,27 @@
       <c r="N1" s="11">
         <v>0</v>
       </c>
-      <c r="O1" s="12">
+      <c r="O1" s="11">
         <v>0</v>
       </c>
       <c r="P1" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q1" s="12">
         <v>1</v>
       </c>
-      <c r="R1" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="R1" s="12">
+        <v>1</v>
+      </c>
+      <c r="S1" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
-        <v>0</v>
-      </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>0</v>
       </c>
       <c r="E2" s="11">
@@ -960,7 +1077,7 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <v>0</v>
       </c>
       <c r="H2" s="12">
@@ -969,10 +1086,10 @@
       <c r="I2" s="12">
         <v>0</v>
       </c>
-      <c r="J2" s="13">
-        <v>0</v>
-      </c>
-      <c r="K2" s="11">
+      <c r="J2" s="12">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13">
         <v>0</v>
       </c>
       <c r="L2" s="11">
@@ -984,28 +1101,29 @@
       <c r="N2" s="11">
         <v>0</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="11">
         <v>0</v>
       </c>
       <c r="P2" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="12">
-        <v>0</v>
-      </c>
-      <c r="R2" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="R2" s="12">
+        <v>0</v>
+      </c>
+      <c r="S2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="B3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="10">
         <v>1</v>
       </c>
       <c r="E3" s="11">
@@ -1014,7 +1132,7 @@
       <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>1</v>
       </c>
       <c r="H3" s="12">
@@ -1023,10 +1141,10 @@
       <c r="I3" s="12">
         <v>1</v>
       </c>
-      <c r="J3" s="13">
-        <v>1</v>
-      </c>
-      <c r="K3" s="11">
+      <c r="J3" s="12">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13">
         <v>1</v>
       </c>
       <c r="L3" s="11">
@@ -1038,30 +1156,31 @@
       <c r="N3" s="11">
         <v>1</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="11">
         <v>1</v>
       </c>
       <c r="P3" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="12">
-        <v>1</v>
-      </c>
-      <c r="R3" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R3" s="12">
+        <v>1</v>
+      </c>
+      <c r="S3" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="16">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="B4" s="2"/>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
         <v>0</v>
       </c>
       <c r="E4" s="11">
@@ -1070,7 +1189,7 @@
       <c r="F4" s="11">
         <v>0</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>0</v>
       </c>
       <c r="H4" s="12">
@@ -1079,10 +1198,10 @@
       <c r="I4" s="12">
         <v>0</v>
       </c>
-      <c r="J4" s="13">
-        <v>0</v>
-      </c>
-      <c r="K4" s="11">
+      <c r="J4" s="12">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
         <v>0</v>
       </c>
       <c r="L4" s="11">
@@ -1094,30 +1213,31 @@
       <c r="N4" s="11">
         <v>0</v>
       </c>
-      <c r="O4" s="12">
-        <v>1</v>
+      <c r="O4" s="11">
+        <v>0</v>
       </c>
       <c r="P4" s="12">
         <v>1</v>
       </c>
       <c r="Q4" s="12">
-        <v>0</v>
-      </c>
-      <c r="R4" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="R4" s="12">
+        <v>0</v>
+      </c>
+      <c r="S4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="B5" s="2"/>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
         <v>1</v>
       </c>
       <c r="E5" s="11">
@@ -1126,7 +1246,7 @@
       <c r="F5" s="11">
         <v>1</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11">
         <v>1</v>
       </c>
       <c r="H5" s="12">
@@ -1135,10 +1255,10 @@
       <c r="I5" s="12">
         <v>1</v>
       </c>
-      <c r="J5" s="13">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11">
+      <c r="J5" s="12">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13">
         <v>1</v>
       </c>
       <c r="L5" s="11">
@@ -1150,187 +1270,191 @@
       <c r="N5" s="11">
         <v>1</v>
       </c>
-      <c r="O5" s="12">
-        <v>0</v>
+      <c r="O5" s="11">
+        <v>1</v>
       </c>
       <c r="P5" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="12">
-        <v>0</v>
-      </c>
-      <c r="R5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="51"/>
-      <c r="AH5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="12">
+        <v>0</v>
+      </c>
+      <c r="S5" s="13">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="51"/>
+      <c r="AI5" s="51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>31</v>
+      </c>
+      <c r="C6" s="9">
         <v>30</v>
       </c>
-      <c r="C6" s="17">
+      <c r="D6" s="17">
         <v>29</v>
       </c>
-      <c r="D6" s="11">
+      <c r="E6" s="11">
         <v>28</v>
       </c>
-      <c r="E6" s="11">
+      <c r="F6" s="11">
         <v>27</v>
       </c>
-      <c r="F6" s="11">
+      <c r="G6" s="11">
         <v>26</v>
       </c>
-      <c r="G6" s="12">
+      <c r="H6" s="12">
         <v>25</v>
       </c>
-      <c r="H6" s="12">
+      <c r="I6" s="12">
         <v>24</v>
       </c>
-      <c r="I6" s="12">
+      <c r="J6" s="12">
         <v>23</v>
       </c>
-      <c r="J6" s="13">
+      <c r="K6" s="13">
         <v>22</v>
       </c>
-      <c r="K6" s="11">
+      <c r="L6" s="11">
         <v>21</v>
       </c>
-      <c r="L6" s="11">
+      <c r="M6" s="11">
         <v>20</v>
       </c>
-      <c r="M6" s="11">
+      <c r="N6" s="11">
         <v>19</v>
       </c>
-      <c r="N6" s="11">
+      <c r="O6" s="11">
         <v>18</v>
       </c>
-      <c r="O6" s="12">
+      <c r="P6" s="12">
         <v>17</v>
       </c>
-      <c r="P6" s="12">
+      <c r="Q6" s="12">
         <v>16</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="R6" s="12">
         <v>15</v>
       </c>
-      <c r="R6" s="13">
+      <c r="S6" s="13">
         <v>14</v>
       </c>
-      <c r="S6" s="11">
+      <c r="T6" s="11">
         <v>13</v>
       </c>
-      <c r="T6" s="11">
+      <c r="U6" s="11">
         <v>12</v>
       </c>
-      <c r="U6" s="11">
+      <c r="V6" s="11">
         <v>11</v>
       </c>
-      <c r="V6" s="11">
+      <c r="W6" s="11">
         <v>10</v>
       </c>
-      <c r="W6" s="12">
+      <c r="X6" s="12">
         <v>9</v>
       </c>
-      <c r="X6" s="12">
+      <c r="Y6" s="12">
         <v>8</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Z6" s="12">
         <v>7</v>
       </c>
-      <c r="Z6" s="12">
+      <c r="AA6" s="12">
         <v>6</v>
       </c>
-      <c r="AA6" s="11">
+      <c r="AB6" s="11">
         <v>5</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AC6" s="11">
         <v>4</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AD6" s="11">
         <v>3</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AE6" s="11">
         <v>2</v>
       </c>
-      <c r="AE6" s="12">
-        <v>1</v>
-      </c>
       <c r="AF6" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="AI6" s="51" t="s">
+      <c r="AJ6" s="51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="16">
+      <c r="B7" s="2"/>
+      <c r="C7" s="16">
         <v>6</v>
       </c>
-      <c r="C7" s="10">
+      <c r="D7" s="10">
         <v>5</v>
       </c>
-      <c r="D7" s="11">
+      <c r="E7" s="11">
         <v>4</v>
       </c>
-      <c r="E7" s="11">
+      <c r="F7" s="11">
         <v>3</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G7" s="11">
         <v>2</v>
       </c>
-      <c r="G7" s="12">
-        <v>1</v>
-      </c>
       <c r="H7" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="12">
+        <v>0</v>
+      </c>
+      <c r="J7" s="12">
         <v>9</v>
       </c>
-      <c r="J7" s="13">
+      <c r="K7" s="13">
         <v>8</v>
       </c>
-      <c r="K7" s="11">
+      <c r="L7" s="11">
         <v>7</v>
       </c>
-      <c r="L7" s="11">
+      <c r="M7" s="11">
         <v>6</v>
       </c>
-      <c r="M7" s="11">
+      <c r="N7" s="11">
         <v>5</v>
       </c>
-      <c r="N7" s="11">
+      <c r="O7" s="11">
         <v>4</v>
       </c>
-      <c r="O7" s="12">
+      <c r="P7" s="12">
         <v>3</v>
       </c>
-      <c r="P7" s="12">
+      <c r="Q7" s="12">
         <v>2</v>
       </c>
-      <c r="Q7" s="12">
-        <v>1</v>
-      </c>
-      <c r="R7" s="13">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="51"/>
-    </row>
-    <row r="8" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="18">
-        <v>0</v>
-      </c>
-      <c r="C8" s="19">
-        <v>0</v>
-      </c>
-      <c r="D8" s="20">
+      <c r="R7" s="12">
+        <v>1</v>
+      </c>
+      <c r="S7" s="13">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="51"/>
+    </row>
+    <row r="8" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="18">
+        <v>0</v>
+      </c>
+      <c r="D8" s="19">
         <v>0</v>
       </c>
       <c r="E8" s="20">
@@ -1339,7 +1463,7 @@
       <c r="F8" s="20">
         <v>0</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>0</v>
       </c>
       <c r="H8" s="21">
@@ -1348,10 +1472,10 @@
       <c r="I8" s="21">
         <v>0</v>
       </c>
-      <c r="J8" s="22">
-        <v>0</v>
-      </c>
-      <c r="K8" s="20">
+      <c r="J8" s="21">
+        <v>0</v>
+      </c>
+      <c r="K8" s="22">
         <v>0</v>
       </c>
       <c r="L8" s="20">
@@ -1363,7 +1487,7 @@
       <c r="N8" s="20">
         <v>0</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="20">
         <v>0</v>
       </c>
       <c r="P8" s="21">
@@ -1372,10 +1496,10 @@
       <c r="Q8" s="21">
         <v>0</v>
       </c>
-      <c r="R8" s="22">
-        <v>0</v>
-      </c>
-      <c r="S8" s="23">
+      <c r="R8" s="21">
+        <v>0</v>
+      </c>
+      <c r="S8" s="22">
         <v>0</v>
       </c>
       <c r="T8" s="23">
@@ -1387,7 +1511,7 @@
       <c r="V8" s="23">
         <v>0</v>
       </c>
-      <c r="W8" s="24">
+      <c r="W8" s="23">
         <v>0</v>
       </c>
       <c r="X8" s="24">
@@ -1399,7 +1523,7 @@
       <c r="Z8" s="24">
         <v>0</v>
       </c>
-      <c r="AA8" s="23">
+      <c r="AA8" s="24">
         <v>0</v>
       </c>
       <c r="AB8" s="23">
@@ -1411,51 +1535,52 @@
       <c r="AD8" s="23">
         <v>0</v>
       </c>
-      <c r="AE8" s="24">
+      <c r="AE8" s="23">
         <v>0</v>
       </c>
       <c r="AF8" s="24">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="83">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="52">
-        <v>1</v>
-      </c>
-      <c r="AI8" s="53">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="79">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="25"/>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="24">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="82">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="52">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="53">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="78">
+        <v>0</v>
+      </c>
       <c r="AL8" s="25"/>
       <c r="AM8" s="25"/>
-      <c r="AN8" s="26"/>
+      <c r="AN8" s="25"/>
       <c r="AO8" s="26"/>
       <c r="AP8" s="26"/>
       <c r="AQ8" s="26"/>
-      <c r="AR8" s="25"/>
+      <c r="AR8" s="26"/>
       <c r="AS8" s="25"/>
       <c r="AT8" s="25"/>
       <c r="AU8" s="25"/>
-      <c r="AV8" s="26"/>
+      <c r="AV8" s="25"/>
       <c r="AW8" s="26"/>
       <c r="AX8" s="26"/>
       <c r="AY8" s="26"/>
-    </row>
-    <row r="9" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AZ8" s="26"/>
+    </row>
+    <row r="9" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="56">
-        <v>0</v>
-      </c>
-      <c r="C9" s="34">
-        <v>0</v>
-      </c>
-      <c r="D9" s="35">
+      <c r="B9" s="55"/>
+      <c r="C9" s="56">
+        <v>0</v>
+      </c>
+      <c r="D9" s="34">
         <v>0</v>
       </c>
       <c r="E9" s="35">
@@ -1464,7 +1589,7 @@
       <c r="F9" s="35">
         <v>0</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="35">
         <v>0</v>
       </c>
       <c r="H9" s="36">
@@ -1473,10 +1598,10 @@
       <c r="I9" s="36">
         <v>0</v>
       </c>
-      <c r="J9" s="37">
-        <v>0</v>
-      </c>
-      <c r="K9" s="35">
+      <c r="J9" s="36">
+        <v>0</v>
+      </c>
+      <c r="K9" s="37">
         <v>0</v>
       </c>
       <c r="L9" s="35">
@@ -1488,60 +1613,60 @@
       <c r="N9" s="35">
         <v>0</v>
       </c>
-      <c r="O9" s="36">
+      <c r="O9" s="35">
         <v>0</v>
       </c>
       <c r="P9" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="36">
         <v>1</v>
       </c>
-      <c r="R9" s="37">
-        <v>0</v>
-      </c>
-      <c r="S9" s="35"/>
-      <c r="T9" s="45"/>
+      <c r="R9" s="36">
+        <v>1</v>
+      </c>
+      <c r="S9" s="37">
+        <v>0</v>
+      </c>
+      <c r="T9" s="35"/>
       <c r="U9" s="45"/>
       <c r="V9" s="45"/>
-      <c r="W9" s="46"/>
+      <c r="W9" s="45"/>
       <c r="X9" s="46"/>
       <c r="Y9" s="46"/>
       <c r="Z9" s="46"/>
-      <c r="AA9" s="45"/>
+      <c r="AA9" s="46"/>
       <c r="AB9" s="45"/>
       <c r="AC9" s="45"/>
       <c r="AD9" s="45"/>
-      <c r="AE9" s="46"/>
+      <c r="AE9" s="45"/>
       <c r="AF9" s="46"/>
-      <c r="AG9" s="84"/>
-      <c r="AH9" s="57"/>
+      <c r="AG9" s="46"/>
+      <c r="AH9" s="83"/>
       <c r="AI9" s="57"/>
-      <c r="AJ9" s="80"/>
-      <c r="AK9" s="38"/>
+      <c r="AJ9" s="57"/>
+      <c r="AK9" s="79"/>
       <c r="AL9" s="38"/>
       <c r="AM9" s="38"/>
-      <c r="AN9" s="39"/>
+      <c r="AN9" s="38"/>
       <c r="AO9" s="39"/>
       <c r="AP9" s="39"/>
       <c r="AQ9" s="39"/>
-      <c r="AR9" s="38"/>
+      <c r="AR9" s="39"/>
       <c r="AS9" s="38"/>
       <c r="AT9" s="38"/>
       <c r="AU9" s="38"/>
-      <c r="AV9" s="39"/>
+      <c r="AV9" s="38"/>
       <c r="AW9" s="39"/>
       <c r="AX9" s="39"/>
       <c r="AY9" s="39"/>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="17">
-        <v>0</v>
-      </c>
-      <c r="D10" s="11">
+      <c r="AZ9" s="39"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="17">
         <v>0</v>
       </c>
       <c r="E10" s="11">
@@ -1550,7 +1675,7 @@
       <c r="F10" s="11">
         <v>0</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <v>0</v>
       </c>
       <c r="H10" s="12">
@@ -1559,10 +1684,10 @@
       <c r="I10" s="12">
         <v>0</v>
       </c>
-      <c r="J10" s="13">
-        <v>0</v>
-      </c>
-      <c r="K10" s="11">
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="13">
         <v>0</v>
       </c>
       <c r="L10" s="11">
@@ -1574,31 +1699,31 @@
       <c r="N10" s="11">
         <v>0</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="11">
         <v>0</v>
       </c>
       <c r="P10" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="12">
         <v>1</v>
       </c>
-      <c r="R10" s="13">
-        <v>0</v>
-      </c>
-      <c r="S10" s="11">
+      <c r="R10" s="12">
+        <v>1</v>
+      </c>
+      <c r="S10" s="13">
         <v>0</v>
       </c>
       <c r="T10" s="11">
         <v>0</v>
       </c>
-      <c r="U10" s="27">
+      <c r="U10" s="11">
         <v>0</v>
       </c>
       <c r="V10" s="27">
         <v>0</v>
       </c>
-      <c r="W10" s="28">
+      <c r="W10" s="27">
         <v>0</v>
       </c>
       <c r="X10" s="28">
@@ -1610,7 +1735,7 @@
       <c r="Z10" s="28">
         <v>0</v>
       </c>
-      <c r="AA10" s="27">
+      <c r="AA10" s="28">
         <v>0</v>
       </c>
       <c r="AB10" s="27">
@@ -1622,37 +1747,38 @@
       <c r="AD10" s="27">
         <v>0</v>
       </c>
-      <c r="AE10" s="28">
+      <c r="AE10" s="27">
         <v>0</v>
       </c>
       <c r="AF10" s="28">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="85">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="54">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="28">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="84">
+        <v>0</v>
       </c>
       <c r="AI10" s="54">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="50">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="29"/>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="54">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="50">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="29"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="17">
-        <v>0</v>
-      </c>
-      <c r="D11" s="11">
+      <c r="B11" s="2"/>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
         <v>0</v>
       </c>
       <c r="E11" s="11">
@@ -1661,7 +1787,7 @@
       <c r="F11" s="11">
         <v>0</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <v>0</v>
       </c>
       <c r="H11" s="12">
@@ -1670,10 +1796,10 @@
       <c r="I11" s="12">
         <v>0</v>
       </c>
-      <c r="J11" s="13">
-        <v>0</v>
-      </c>
-      <c r="K11" s="11">
+      <c r="J11" s="12">
+        <v>0</v>
+      </c>
+      <c r="K11" s="13">
         <v>0</v>
       </c>
       <c r="L11" s="11">
@@ -1685,7 +1811,7 @@
       <c r="N11" s="11">
         <v>0</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="11">
         <v>0</v>
       </c>
       <c r="P11" s="12">
@@ -1694,22 +1820,22 @@
       <c r="Q11" s="12">
         <v>0</v>
       </c>
-      <c r="R11" s="13">
-        <v>1</v>
-      </c>
-      <c r="S11" s="11">
+      <c r="R11" s="12">
+        <v>0</v>
+      </c>
+      <c r="S11" s="13">
         <v>1</v>
       </c>
       <c r="T11" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="11">
         <v>0</v>
       </c>
-      <c r="V11" s="60">
-        <v>0</v>
-      </c>
-      <c r="W11" s="28">
+      <c r="V11" s="11">
+        <v>0</v>
+      </c>
+      <c r="W11" s="60">
         <v>0</v>
       </c>
       <c r="X11" s="28">
@@ -1721,7 +1847,7 @@
       <c r="Z11" s="28">
         <v>0</v>
       </c>
-      <c r="AA11" s="27">
+      <c r="AA11" s="28">
         <v>0</v>
       </c>
       <c r="AB11" s="27">
@@ -1733,42 +1859,43 @@
       <c r="AD11" s="27">
         <v>0</v>
       </c>
-      <c r="AE11" s="28">
+      <c r="AE11" s="27">
         <v>0</v>
       </c>
       <c r="AF11" s="28">
         <v>0</v>
       </c>
-      <c r="AG11" s="85">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="54">
-        <v>1</v>
+      <c r="AG11" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="84">
+        <v>0</v>
       </c>
       <c r="AI11" s="54">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="50">
-        <v>1</v>
-      </c>
-      <c r="AK11" s="30">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="54">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="50">
+        <v>1</v>
       </c>
       <c r="AL11" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AM11" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="56">
-        <v>0</v>
-      </c>
-      <c r="C12" s="34">
-        <v>0</v>
-      </c>
-      <c r="D12" s="35">
+      <c r="B12" s="2"/>
+      <c r="C12" s="56">
+        <v>0</v>
+      </c>
+      <c r="D12" s="34">
         <v>0</v>
       </c>
       <c r="E12" s="35">
@@ -1777,7 +1904,7 @@
       <c r="F12" s="35">
         <v>0</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="35">
         <v>0</v>
       </c>
       <c r="H12" s="36">
@@ -1786,10 +1913,10 @@
       <c r="I12" s="36">
         <v>0</v>
       </c>
-      <c r="J12" s="37">
-        <v>0</v>
-      </c>
-      <c r="K12" s="35">
+      <c r="J12" s="36">
+        <v>0</v>
+      </c>
+      <c r="K12" s="37">
         <v>0</v>
       </c>
       <c r="L12" s="35">
@@ -1801,27 +1928,27 @@
       <c r="N12" s="35">
         <v>0</v>
       </c>
-      <c r="O12" s="36">
+      <c r="O12" s="35">
         <v>0</v>
       </c>
       <c r="P12" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="36">
         <v>1</v>
       </c>
-      <c r="R12" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18">
-        <v>0</v>
-      </c>
-      <c r="C13" s="19">
-        <v>0</v>
-      </c>
-      <c r="D13" s="20">
+      <c r="R12" s="36">
+        <v>1</v>
+      </c>
+      <c r="S12" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="18">
+        <v>0</v>
+      </c>
+      <c r="D13" s="19">
         <v>0</v>
       </c>
       <c r="E13" s="20">
@@ -1830,7 +1957,7 @@
       <c r="F13" s="20">
         <v>0</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="20">
         <v>0</v>
       </c>
       <c r="H13" s="21">
@@ -1839,10 +1966,10 @@
       <c r="I13" s="21">
         <v>0</v>
       </c>
-      <c r="J13" s="22">
-        <v>0</v>
-      </c>
-      <c r="K13" s="20">
+      <c r="J13" s="21">
+        <v>0</v>
+      </c>
+      <c r="K13" s="22">
         <v>0</v>
       </c>
       <c r="L13" s="20">
@@ -1854,31 +1981,31 @@
       <c r="N13" s="20">
         <v>0</v>
       </c>
-      <c r="O13" s="21">
+      <c r="O13" s="20">
         <v>0</v>
       </c>
       <c r="P13" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="21">
         <v>1</v>
       </c>
-      <c r="R13" s="22">
-        <v>1</v>
-      </c>
-      <c r="S13" s="20">
+      <c r="R13" s="21">
+        <v>1</v>
+      </c>
+      <c r="S13" s="22">
         <v>1</v>
       </c>
       <c r="T13" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="20">
         <v>0</v>
       </c>
-      <c r="V13" s="61">
-        <v>0</v>
-      </c>
-      <c r="W13" s="24">
+      <c r="V13" s="20">
+        <v>0</v>
+      </c>
+      <c r="W13" s="61">
         <v>0</v>
       </c>
       <c r="X13" s="24">
@@ -1890,7 +2017,7 @@
       <c r="Z13" s="24">
         <v>0</v>
       </c>
-      <c r="AA13" s="23">
+      <c r="AA13" s="24">
         <v>0</v>
       </c>
       <c r="AB13" s="23">
@@ -1902,55 +2029,56 @@
       <c r="AD13" s="23">
         <v>0</v>
       </c>
-      <c r="AE13" s="24">
+      <c r="AE13" s="23">
         <v>0</v>
       </c>
       <c r="AF13" s="24">
         <v>0</v>
       </c>
-      <c r="AG13" s="83">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="52">
-        <v>1</v>
+      <c r="AG13" s="24">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="82">
+        <v>0</v>
       </c>
       <c r="AI13" s="52">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="49">
-        <v>1</v>
-      </c>
-      <c r="AK13" s="31">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="52">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="49">
+        <v>1</v>
       </c>
       <c r="AL13" s="31">
         <v>0</v>
       </c>
-      <c r="AM13" s="25"/>
-      <c r="AN13" s="26"/>
+      <c r="AM13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="25"/>
       <c r="AO13" s="26"/>
       <c r="AP13" s="26"/>
       <c r="AQ13" s="26"/>
-      <c r="AR13" s="25"/>
+      <c r="AR13" s="26"/>
       <c r="AS13" s="25"/>
       <c r="AT13" s="25"/>
       <c r="AU13" s="25"/>
-      <c r="AV13" s="26"/>
+      <c r="AV13" s="25"/>
       <c r="AW13" s="26"/>
       <c r="AX13" s="26"/>
       <c r="AY13" s="26"/>
-    </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ13" s="26"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="9">
-        <v>0</v>
-      </c>
-      <c r="C14" s="17">
-        <v>0</v>
-      </c>
-      <c r="D14" s="11">
+      <c r="B14" s="2"/>
+      <c r="C14" s="9">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17">
         <v>0</v>
       </c>
       <c r="E14" s="11">
@@ -1959,7 +2087,7 @@
       <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="11">
         <v>0</v>
       </c>
       <c r="H14" s="12">
@@ -1968,10 +2096,10 @@
       <c r="I14" s="12">
         <v>0</v>
       </c>
-      <c r="J14" s="13">
-        <v>0</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
         <v>0</v>
       </c>
       <c r="L14" s="11">
@@ -1983,7 +2111,7 @@
       <c r="N14" s="11">
         <v>0</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="11">
         <v>0</v>
       </c>
       <c r="P14" s="12">
@@ -1992,10 +2120,10 @@
       <c r="Q14" s="12">
         <v>0</v>
       </c>
-      <c r="R14" s="13">
-        <v>1</v>
-      </c>
-      <c r="S14" s="11">
+      <c r="R14" s="12">
+        <v>0</v>
+      </c>
+      <c r="S14" s="13">
         <v>1</v>
       </c>
       <c r="T14" s="11">
@@ -2005,21 +2133,21 @@
         <v>1</v>
       </c>
       <c r="V14" s="11">
-        <v>0</v>
-      </c>
-      <c r="W14" s="62">
+        <v>1</v>
+      </c>
+      <c r="W14" s="11">
         <v>0</v>
       </c>
       <c r="X14" s="62">
         <v>0</v>
       </c>
-      <c r="Y14" s="28">
+      <c r="Y14" s="62">
         <v>0</v>
       </c>
       <c r="Z14" s="28">
         <v>0</v>
       </c>
-      <c r="AA14" s="27">
+      <c r="AA14" s="28">
         <v>0</v>
       </c>
       <c r="AB14" s="27">
@@ -2031,51 +2159,52 @@
       <c r="AD14" s="27">
         <v>0</v>
       </c>
-      <c r="AE14" s="28">
+      <c r="AE14" s="27">
         <v>0</v>
       </c>
       <c r="AF14" s="28">
         <v>0</v>
       </c>
-      <c r="AG14" s="85">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="54">
+      <c r="AG14" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="84">
         <v>0</v>
       </c>
       <c r="AI14" s="54">
         <v>0</v>
       </c>
-      <c r="AJ14" s="50">
-        <v>1</v>
-      </c>
-      <c r="AK14" s="30">
-        <v>0</v>
+      <c r="AJ14" s="54">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="50">
+        <v>1</v>
       </c>
       <c r="AL14" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="30">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35">
-        <v>0</v>
-      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="35">
         <v>0</v>
       </c>
       <c r="F15" s="35">
         <v>0</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="35">
         <v>0</v>
       </c>
       <c r="H15" s="36">
@@ -2084,10 +2213,10 @@
       <c r="I15" s="36">
         <v>0</v>
       </c>
-      <c r="J15" s="37">
-        <v>0</v>
-      </c>
-      <c r="K15" s="35">
+      <c r="J15" s="36">
+        <v>0</v>
+      </c>
+      <c r="K15" s="37">
         <v>0</v>
       </c>
       <c r="L15" s="35">
@@ -2099,7 +2228,7 @@
       <c r="N15" s="35">
         <v>0</v>
       </c>
-      <c r="O15" s="36">
+      <c r="O15" s="35">
         <v>0</v>
       </c>
       <c r="P15" s="36">
@@ -2108,14 +2237,14 @@
       <c r="Q15" s="36">
         <v>0</v>
       </c>
-      <c r="R15" s="37">
-        <v>0</v>
-      </c>
-      <c r="S15" s="35">
+      <c r="R15" s="36">
+        <v>0</v>
+      </c>
+      <c r="S15" s="37">
         <v>0</v>
       </c>
       <c r="T15" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="35">
         <v>1</v>
@@ -2123,11 +2252,11 @@
       <c r="V15" s="35">
         <v>1</v>
       </c>
-      <c r="W15" s="36">
-        <v>1</v>
-      </c>
-      <c r="X15" s="46">
-        <v>0</v>
+      <c r="W15" s="35">
+        <v>1</v>
+      </c>
+      <c r="X15" s="36">
+        <v>1</v>
       </c>
       <c r="Y15" s="46">
         <v>0</v>
@@ -2135,7 +2264,7 @@
       <c r="Z15" s="46">
         <v>0</v>
       </c>
-      <c r="AA15" s="45">
+      <c r="AA15" s="46">
         <v>0</v>
       </c>
       <c r="AB15" s="45">
@@ -2147,57 +2276,57 @@
       <c r="AD15" s="45">
         <v>0</v>
       </c>
-      <c r="AE15" s="46">
+      <c r="AE15" s="45">
         <v>0</v>
       </c>
       <c r="AF15" s="46">
         <v>0</v>
       </c>
-      <c r="AG15" s="84">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="57">
+      <c r="AG15" s="46">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="83">
         <v>0</v>
       </c>
       <c r="AI15" s="57">
         <v>0</v>
       </c>
-      <c r="AJ15" s="80">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="58">
+      <c r="AJ15" s="57">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="79">
         <v>0</v>
       </c>
       <c r="AL15" s="58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="58">
-        <v>0</v>
-      </c>
-      <c r="AN15" s="59">
-        <v>1</v>
-      </c>
-      <c r="AO15" s="39">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AN15" s="58">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="59">
+        <v>1</v>
       </c>
       <c r="AP15" s="39">
         <v>0</v>
       </c>
-      <c r="AQ15" s="39"/>
-      <c r="AR15" s="38"/>
+      <c r="AQ15" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="39"/>
       <c r="AS15" s="38"/>
       <c r="AT15" s="38"/>
       <c r="AU15" s="38"/>
-      <c r="AV15" s="39"/>
+      <c r="AV15" s="38"/>
       <c r="AW15" s="39"/>
       <c r="AX15" s="39"/>
       <c r="AY15" s="39"/>
-    </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="F16" s="11">
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="AZ15" s="39"/>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="G16" s="11">
         <v>0</v>
       </c>
       <c r="H16" s="12">
@@ -2206,10 +2335,10 @@
       <c r="I16" s="12">
         <v>0</v>
       </c>
-      <c r="J16" s="13">
-        <v>0</v>
-      </c>
-      <c r="K16" s="11">
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="13">
         <v>0</v>
       </c>
       <c r="L16" s="11">
@@ -2221,7 +2350,7 @@
       <c r="N16" s="11">
         <v>0</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="11">
         <v>0</v>
       </c>
       <c r="P16" s="12">
@@ -2230,10 +2359,10 @@
       <c r="Q16" s="12">
         <v>0</v>
       </c>
-      <c r="R16" s="13">
-        <v>0</v>
-      </c>
-      <c r="S16" s="11">
+      <c r="R16" s="12">
+        <v>0</v>
+      </c>
+      <c r="S16" s="13">
         <v>0</v>
       </c>
       <c r="T16" s="11">
@@ -2243,21 +2372,21 @@
         <v>0</v>
       </c>
       <c r="V16" s="11">
-        <v>1</v>
-      </c>
-      <c r="W16" s="12">
+        <v>0</v>
+      </c>
+      <c r="W16" s="11">
         <v>1</v>
       </c>
       <c r="X16" s="12">
         <v>1</v>
       </c>
-      <c r="Y16" s="28">
+      <c r="Y16" s="12">
         <v>1</v>
       </c>
       <c r="Z16" s="28">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="28">
         <v>0</v>
       </c>
       <c r="AB16" s="27">
@@ -2269,25 +2398,25 @@
       <c r="AD16" s="27">
         <v>0</v>
       </c>
-      <c r="AE16" s="28">
+      <c r="AE16" s="27">
         <v>0</v>
       </c>
       <c r="AF16" s="28">
         <v>0</v>
       </c>
-      <c r="AG16" s="85">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="54">
+      <c r="AG16" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="84">
         <v>0</v>
       </c>
       <c r="AI16" s="54">
         <v>0</v>
       </c>
-      <c r="AJ16" s="50">
-        <v>0</v>
-      </c>
-      <c r="AK16" s="30">
+      <c r="AJ16" s="54">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="50">
         <v>0</v>
       </c>
       <c r="AL16" s="30">
@@ -2296,36 +2425,37 @@
       <c r="AM16" s="30">
         <v>0</v>
       </c>
-      <c r="AN16" s="32">
-        <v>1</v>
+      <c r="AN16" s="30">
+        <v>0</v>
       </c>
       <c r="AO16" s="32">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="15">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="AP16" s="32">
+        <v>0</v>
       </c>
       <c r="AQ16" s="15">
-        <v>0</v>
-      </c>
-      <c r="AR16" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="12">
-        <v>0</v>
-      </c>
+      <c r="B17" s="4"/>
       <c r="I17" s="12">
         <v>0</v>
       </c>
-      <c r="J17" s="13">
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="13">
         <v>0</v>
       </c>
       <c r="L17" s="11">
@@ -2337,7 +2467,7 @@
       <c r="N17" s="11">
         <v>0</v>
       </c>
-      <c r="O17" s="12">
+      <c r="O17" s="11">
         <v>0</v>
       </c>
       <c r="P17" s="12">
@@ -2346,10 +2476,10 @@
       <c r="Q17" s="12">
         <v>0</v>
       </c>
-      <c r="R17" s="13">
-        <v>0</v>
-      </c>
-      <c r="S17" s="11">
+      <c r="R17" s="12">
+        <v>0</v>
+      </c>
+      <c r="S17" s="13">
         <v>0</v>
       </c>
       <c r="T17" s="11">
@@ -2361,23 +2491,23 @@
       <c r="V17" s="11">
         <v>0</v>
       </c>
-      <c r="W17" s="12">
+      <c r="W17" s="11">
         <v>0</v>
       </c>
       <c r="X17" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="12">
         <v>1</v>
       </c>
-      <c r="Z17" s="62">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="27">
+      <c r="Z17" s="12">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="62">
         <v>1</v>
       </c>
       <c r="AB17" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC17" s="27">
         <v>0</v>
@@ -2385,25 +2515,25 @@
       <c r="AD17" s="27">
         <v>0</v>
       </c>
-      <c r="AE17" s="28">
+      <c r="AE17" s="27">
         <v>0</v>
       </c>
       <c r="AF17" s="28">
         <v>0</v>
       </c>
-      <c r="AG17" s="85">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="54">
+      <c r="AG17" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="84">
         <v>0</v>
       </c>
       <c r="AI17" s="54">
         <v>0</v>
       </c>
-      <c r="AJ17" s="50">
-        <v>0</v>
-      </c>
-      <c r="AK17" s="30">
+      <c r="AJ17" s="54">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="50">
         <v>0</v>
       </c>
       <c r="AL17" s="30">
@@ -2412,44 +2542,45 @@
       <c r="AM17" s="30">
         <v>0</v>
       </c>
-      <c r="AN17" s="32">
+      <c r="AN17" s="30">
         <v>0</v>
       </c>
       <c r="AO17" s="32">
         <v>0</v>
       </c>
       <c r="AP17" s="32">
-        <v>1</v>
-      </c>
-      <c r="AQ17" s="15">
-        <v>0</v>
-      </c>
-      <c r="AR17" s="14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="32">
+        <v>1</v>
+      </c>
+      <c r="AR17" s="15">
+        <v>0</v>
       </c>
       <c r="AS17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT17" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AU17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:52" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="11"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
-      <c r="J18" s="13">
-        <v>0</v>
-      </c>
-      <c r="K18" s="11">
+      <c r="J18" s="12"/>
+      <c r="K18" s="13">
         <v>0</v>
       </c>
       <c r="L18" s="11">
@@ -2461,7 +2592,7 @@
       <c r="N18" s="11">
         <v>0</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="11">
         <v>0</v>
       </c>
       <c r="P18" s="12">
@@ -2470,10 +2601,10 @@
       <c r="Q18" s="12">
         <v>0</v>
       </c>
-      <c r="R18" s="13">
-        <v>0</v>
-      </c>
-      <c r="S18" s="11">
+      <c r="R18" s="12">
+        <v>0</v>
+      </c>
+      <c r="S18" s="13">
         <v>0</v>
       </c>
       <c r="T18" s="11">
@@ -2485,7 +2616,7 @@
       <c r="V18" s="11">
         <v>0</v>
       </c>
-      <c r="W18" s="12">
+      <c r="W18" s="11">
         <v>0</v>
       </c>
       <c r="X18" s="12">
@@ -2495,39 +2626,39 @@
         <v>0</v>
       </c>
       <c r="Z18" s="12">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="12">
         <v>1</v>
       </c>
       <c r="AB18" s="11">
         <v>1</v>
       </c>
-      <c r="AC18" s="27">
+      <c r="AC18" s="11">
         <v>1</v>
       </c>
       <c r="AD18" s="27">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="28">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="27">
         <v>0</v>
       </c>
       <c r="AF18" s="28">
         <v>0</v>
       </c>
-      <c r="AG18" s="86">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="64">
+      <c r="AG18" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="85">
         <v>0</v>
       </c>
       <c r="AI18" s="64">
         <v>0</v>
       </c>
-      <c r="AJ18" s="81">
-        <v>0</v>
-      </c>
-      <c r="AK18" s="29">
+      <c r="AJ18" s="64">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="80">
         <v>0</v>
       </c>
       <c r="AL18" s="29">
@@ -2536,7 +2667,7 @@
       <c r="AM18" s="29">
         <v>0</v>
       </c>
-      <c r="AN18" s="65">
+      <c r="AN18" s="29">
         <v>0</v>
       </c>
       <c r="AO18" s="65">
@@ -2548,39 +2679,40 @@
       <c r="AQ18" s="65">
         <v>0</v>
       </c>
-      <c r="AR18" s="29">
-        <v>1</v>
-      </c>
-      <c r="AS18" s="38">
-        <v>0</v>
+      <c r="AR18" s="65">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="29">
+        <v>1</v>
       </c>
       <c r="AT18" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU18" s="38">
-        <v>0</v>
-      </c>
-      <c r="AV18" s="39">
-        <v>0</v>
-      </c>
-      <c r="AW18" s="39"/>
+        <v>1</v>
+      </c>
+      <c r="AV18" s="38">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="39">
+        <v>0</v>
+      </c>
       <c r="AX18" s="39"/>
       <c r="AY18" s="39"/>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ18" s="39"/>
+    </row>
+    <row r="19" spans="1:52" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L19" s="11">
-        <v>0</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="M19" s="11">
         <v>0</v>
       </c>
       <c r="N19" s="11">
         <v>0</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="11">
         <v>0</v>
       </c>
       <c r="P19" s="12">
@@ -2589,10 +2721,10 @@
       <c r="Q19" s="12">
         <v>0</v>
       </c>
-      <c r="R19" s="13">
-        <v>0</v>
-      </c>
-      <c r="S19" s="11">
+      <c r="R19" s="12">
+        <v>0</v>
+      </c>
+      <c r="S19" s="13">
         <v>0</v>
       </c>
       <c r="T19" s="11">
@@ -2604,7 +2736,7 @@
       <c r="V19" s="11">
         <v>0</v>
       </c>
-      <c r="W19" s="12">
+      <c r="W19" s="11">
         <v>0</v>
       </c>
       <c r="X19" s="12">
@@ -2613,14 +2745,14 @@
       <c r="Y19" s="12">
         <v>0</v>
       </c>
-      <c r="Z19" s="62">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="60">
+      <c r="Z19" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="62">
         <v>0</v>
       </c>
       <c r="AB19" s="60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="60">
         <v>1</v>
@@ -2628,25 +2760,25 @@
       <c r="AD19" s="60">
         <v>1</v>
       </c>
-      <c r="AE19" s="28">
+      <c r="AE19" s="60">
         <v>1</v>
       </c>
       <c r="AF19" s="28">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="85">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="54">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="28">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="84">
         <v>0</v>
       </c>
       <c r="AI19" s="54">
         <v>0</v>
       </c>
-      <c r="AJ19" s="50">
-        <v>0</v>
-      </c>
-      <c r="AK19" s="30">
+      <c r="AJ19" s="54">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="50">
         <v>0</v>
       </c>
       <c r="AL19" s="30">
@@ -2655,7 +2787,7 @@
       <c r="AM19" s="30">
         <v>0</v>
       </c>
-      <c r="AN19" s="32">
+      <c r="AN19" s="30">
         <v>0</v>
       </c>
       <c r="AO19" s="32">
@@ -2667,559 +2799,675 @@
       <c r="AQ19" s="32">
         <v>0</v>
       </c>
-      <c r="AR19" s="30">
+      <c r="AR19" s="32">
         <v>0</v>
       </c>
       <c r="AS19" s="30">
         <v>0</v>
       </c>
       <c r="AT19" s="30">
-        <v>1</v>
-      </c>
-      <c r="AU19" s="14">
-        <v>0</v>
-      </c>
-      <c r="AV19" s="15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AU19" s="30">
+        <v>1</v>
+      </c>
+      <c r="AV19" s="14">
+        <v>0</v>
       </c>
       <c r="AW19" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX19" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:51" s="73" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="72"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="60"/>
-      <c r="U20" s="60"/>
-      <c r="V20" s="60"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="60"/>
-      <c r="AB20" s="60"/>
-      <c r="AC20" s="60"/>
-      <c r="AD20" s="60"/>
-      <c r="AE20" s="62"/>
-      <c r="AF20" s="62"/>
-      <c r="AG20" s="85"/>
-      <c r="AH20" s="54"/>
+      <c r="AY19" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:52" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="94" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="95">
+        <v>0</v>
+      </c>
+      <c r="C20" s="96">
+        <v>0</v>
+      </c>
+      <c r="D20" s="97">
+        <v>0</v>
+      </c>
+      <c r="E20" s="98">
+        <v>0</v>
+      </c>
+      <c r="F20" s="98">
+        <v>0</v>
+      </c>
+      <c r="G20" s="98">
+        <v>0</v>
+      </c>
+      <c r="H20" s="99">
+        <v>0</v>
+      </c>
+      <c r="I20" s="99">
+        <v>0</v>
+      </c>
+      <c r="J20" s="99">
+        <v>0</v>
+      </c>
+      <c r="K20" s="100">
+        <v>0</v>
+      </c>
+      <c r="L20" s="98">
+        <v>0</v>
+      </c>
+      <c r="M20" s="98">
+        <v>0</v>
+      </c>
+      <c r="N20" s="98">
+        <v>0</v>
+      </c>
+      <c r="O20" s="98">
+        <v>0</v>
+      </c>
+      <c r="P20" s="99">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="99">
+        <v>0</v>
+      </c>
+      <c r="R20" s="99">
+        <v>0</v>
+      </c>
+      <c r="S20" s="100">
+        <v>0</v>
+      </c>
+      <c r="T20" s="98">
+        <v>0</v>
+      </c>
+      <c r="U20" s="98">
+        <v>0</v>
+      </c>
+      <c r="V20" s="98">
+        <v>0</v>
+      </c>
+      <c r="W20" s="98">
+        <v>0</v>
+      </c>
+      <c r="X20" s="99">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="99">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="99">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="99">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="98">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="98">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="98">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="98">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="99">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="101">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="87"/>
       <c r="AI20" s="54"/>
-      <c r="AJ20" s="50"/>
-      <c r="AK20" s="30"/>
+      <c r="AJ20" s="54"/>
+      <c r="AK20" s="50"/>
       <c r="AL20" s="30"/>
       <c r="AM20" s="30"/>
-      <c r="AN20" s="32"/>
+      <c r="AN20" s="30"/>
       <c r="AO20" s="32"/>
       <c r="AP20" s="32"/>
       <c r="AQ20" s="32"/>
-      <c r="AR20" s="30"/>
+      <c r="AR20" s="32"/>
       <c r="AS20" s="30"/>
       <c r="AT20" s="30"/>
       <c r="AU20" s="30"/>
-      <c r="AV20" s="32"/>
-      <c r="AW20" s="67"/>
+      <c r="AV20" s="30"/>
+      <c r="AW20" s="32"/>
       <c r="AX20" s="67"/>
       <c r="AY20" s="67"/>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="AH21" s="54"/>
+      <c r="AZ20" s="67"/>
+    </row>
+    <row r="21" spans="1:52" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="102"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="106"/>
+      <c r="N21" s="106"/>
+      <c r="O21" s="106"/>
+      <c r="P21" s="107"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="107"/>
+      <c r="S21" s="108"/>
+      <c r="T21" s="106"/>
+      <c r="U21" s="106"/>
+      <c r="V21" s="106"/>
+      <c r="W21" s="106"/>
+      <c r="X21" s="107"/>
+      <c r="Y21" s="107"/>
+      <c r="Z21" s="107"/>
+      <c r="AA21" s="107"/>
+      <c r="AB21" s="106"/>
+      <c r="AC21" s="106"/>
+      <c r="AD21" s="106"/>
+      <c r="AE21" s="106"/>
+      <c r="AF21" s="107"/>
+      <c r="AG21" s="109"/>
+      <c r="AH21" s="90"/>
       <c r="AI21" s="54"/>
-      <c r="AJ21" s="50"/>
-      <c r="AK21" s="30"/>
+      <c r="AJ21" s="54"/>
+      <c r="AK21" s="50"/>
       <c r="AL21" s="30"/>
       <c r="AM21" s="30"/>
-      <c r="AN21" s="32"/>
+      <c r="AN21" s="30"/>
       <c r="AO21" s="32"/>
       <c r="AP21" s="32"/>
       <c r="AQ21" s="32"/>
-      <c r="AR21" s="30"/>
+      <c r="AR21" s="32"/>
       <c r="AS21" s="30"/>
       <c r="AT21" s="30"/>
       <c r="AU21" s="30"/>
-      <c r="AV21" s="32"/>
+      <c r="AV21" s="30"/>
       <c r="AW21" s="32"/>
-    </row>
-    <row r="22" spans="1:51" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AX21" s="32"/>
+    </row>
+    <row r="22" spans="1:52" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="91"/>
-      <c r="B22" s="92"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="94"/>
-      <c r="J22" s="95"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="88"/>
       <c r="K22" s="93"/>
-      <c r="L22" s="93"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="94"/>
-      <c r="R22" s="95"/>
-      <c r="S22" s="90"/>
-      <c r="T22" s="90"/>
-      <c r="U22" s="69"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="89"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="69"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="87"/>
+      <c r="R22" s="88"/>
+      <c r="S22" s="93"/>
+      <c r="T22" s="89"/>
+      <c r="U22" s="89"/>
       <c r="V22" s="69"/>
-      <c r="W22" s="88"/>
-      <c r="X22" s="88"/>
-      <c r="Y22" s="89"/>
-      <c r="Z22" s="89"/>
-      <c r="AA22" s="90"/>
-      <c r="AB22" s="90"/>
-      <c r="AC22" s="69"/>
+      <c r="W22" s="69"/>
+      <c r="X22" s="87"/>
+      <c r="Y22" s="87"/>
+      <c r="Z22" s="88"/>
+      <c r="AA22" s="88"/>
+      <c r="AB22" s="89"/>
+      <c r="AC22" s="89"/>
       <c r="AD22" s="69"/>
-      <c r="AE22" s="88"/>
-      <c r="AF22" s="88"/>
-      <c r="AG22" s="85"/>
-      <c r="AH22" s="51"/>
+      <c r="AE22" s="69"/>
+      <c r="AF22" s="87"/>
+      <c r="AG22" s="87"/>
+      <c r="AH22" s="84"/>
       <c r="AI22" s="51"/>
-      <c r="AJ22" s="78"/>
-      <c r="AK22" s="66"/>
+      <c r="AJ22" s="51"/>
+      <c r="AK22" s="77"/>
       <c r="AL22" s="66"/>
       <c r="AM22" s="66"/>
-      <c r="AN22" s="67"/>
+      <c r="AN22" s="66"/>
       <c r="AO22" s="67"/>
       <c r="AP22" s="67"/>
       <c r="AQ22" s="67"/>
-      <c r="AR22" s="76"/>
-      <c r="AS22" s="76"/>
-      <c r="AT22" s="76"/>
-      <c r="AU22" s="76"/>
-      <c r="AV22" s="77"/>
-      <c r="AW22" s="77"/>
-      <c r="AX22" s="77"/>
-      <c r="AY22" s="77"/>
-    </row>
-    <row r="23" spans="1:51" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AR22" s="67"/>
+      <c r="AS22" s="75"/>
+      <c r="AT22" s="75"/>
+      <c r="AU22" s="75"/>
+      <c r="AV22" s="75"/>
+      <c r="AW22" s="76"/>
+      <c r="AX22" s="76"/>
+      <c r="AY22" s="76"/>
+      <c r="AZ22" s="76"/>
+    </row>
+    <row r="23" spans="1:52" s="73" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="60"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="71"/>
       <c r="E23" s="60"/>
       <c r="F23" s="60"/>
-      <c r="G23" s="62"/>
+      <c r="G23" s="60"/>
       <c r="H23" s="62"/>
       <c r="I23" s="62"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="60"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="72"/>
       <c r="L23" s="60"/>
       <c r="M23" s="60"/>
       <c r="N23" s="60"/>
-      <c r="O23" s="62"/>
+      <c r="O23" s="60"/>
       <c r="P23" s="62"/>
       <c r="Q23" s="62"/>
-      <c r="R23" s="72"/>
-      <c r="S23" s="60"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="72"/>
       <c r="T23" s="60"/>
       <c r="U23" s="60"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="62"/>
+      <c r="W23" s="60"/>
       <c r="X23" s="62"/>
       <c r="Y23" s="62"/>
       <c r="Z23" s="62"/>
-      <c r="AA23" s="60">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="60" t="s">
+      <c r="AA23" s="62"/>
+      <c r="AB23" s="60">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="AC23" s="60"/>
       <c r="AD23" s="60"/>
-      <c r="AE23" s="62"/>
+      <c r="AE23" s="60"/>
       <c r="AF23" s="62"/>
-      <c r="AG23" s="82"/>
-      <c r="AH23" s="51"/>
+      <c r="AG23" s="62"/>
+      <c r="AH23" s="81"/>
       <c r="AI23" s="51"/>
-      <c r="AJ23" s="78"/>
-      <c r="AK23" s="66"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="77"/>
       <c r="AL23" s="66"/>
       <c r="AM23" s="66"/>
-      <c r="AN23" s="67"/>
+      <c r="AN23" s="66"/>
       <c r="AO23" s="67"/>
       <c r="AP23" s="67"/>
       <c r="AQ23" s="67"/>
-      <c r="AR23" s="66"/>
+      <c r="AR23" s="67"/>
       <c r="AS23" s="66"/>
       <c r="AT23" s="66"/>
       <c r="AU23" s="66"/>
-      <c r="AV23" s="67"/>
+      <c r="AV23" s="66"/>
       <c r="AW23" s="67"/>
       <c r="AX23" s="67"/>
       <c r="AY23" s="67"/>
-    </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ23" s="67"/>
+    </row>
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="J25" s="12"/>
-      <c r="AB25" s="27"/>
+      <c r="B24" s="4"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="K25" s="12"/>
       <c r="AC25" s="27"/>
       <c r="AD25" s="27"/>
-      <c r="AE25" s="28"/>
+      <c r="AE25" s="27"/>
       <c r="AF25" s="28"/>
-      <c r="AG25" s="85"/>
-      <c r="AH25" s="54"/>
+      <c r="AG25" s="28"/>
+      <c r="AH25" s="84"/>
       <c r="AI25" s="54"/>
-      <c r="AJ25" s="50"/>
-      <c r="AK25" s="30"/>
+      <c r="AJ25" s="54"/>
+      <c r="AK25" s="50"/>
       <c r="AL25" s="30"/>
       <c r="AM25" s="30"/>
-      <c r="AN25" s="32"/>
+      <c r="AN25" s="30"/>
       <c r="AO25" s="32"/>
       <c r="AP25" s="32"/>
       <c r="AQ25" s="32"/>
-      <c r="AR25" s="30"/>
-    </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AR25" s="32"/>
+      <c r="AS25" s="30"/>
+    </row>
+    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="J26" s="12"/>
-      <c r="AC26" s="27"/>
+      <c r="B26" s="4"/>
+      <c r="K26" s="12"/>
       <c r="AD26" s="27"/>
-      <c r="AE26" s="28"/>
+      <c r="AE26" s="27"/>
       <c r="AF26" s="28"/>
-      <c r="AG26" s="85"/>
-      <c r="AH26" s="54"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="84"/>
       <c r="AI26" s="54"/>
-      <c r="AJ26" s="50"/>
-      <c r="AK26" s="30"/>
+      <c r="AJ26" s="54"/>
+      <c r="AK26" s="50"/>
       <c r="AL26" s="30"/>
       <c r="AM26" s="30"/>
-      <c r="AN26" s="32"/>
+      <c r="AN26" s="30"/>
       <c r="AO26" s="32"/>
       <c r="AP26" s="32"/>
       <c r="AQ26" s="32"/>
-      <c r="AR26" s="30"/>
+      <c r="AR26" s="32"/>
       <c r="AS26" s="30"/>
-    </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AT26" s="30"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="11"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="17"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="12"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
-      <c r="K28" s="11"/>
+      <c r="K28" s="12"/>
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
       <c r="N28" s="11"/>
-      <c r="O28" s="12"/>
+      <c r="O28" s="11"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="11"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="13"/>
       <c r="T28" s="11"/>
       <c r="U28" s="11"/>
       <c r="V28" s="11"/>
-      <c r="W28" s="12"/>
+      <c r="W28" s="11"/>
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
-      <c r="AA28" s="11"/>
+      <c r="AA28" s="12"/>
       <c r="AB28" s="11"/>
-      <c r="AC28" s="27"/>
+      <c r="AC28" s="11"/>
       <c r="AD28" s="27"/>
-      <c r="AE28" s="28"/>
+      <c r="AE28" s="27"/>
       <c r="AF28" s="28"/>
-      <c r="AG28" s="85"/>
-      <c r="AH28" s="54"/>
+      <c r="AG28" s="28"/>
+      <c r="AH28" s="84"/>
       <c r="AI28" s="54"/>
-      <c r="AJ28" s="50"/>
-      <c r="AK28" s="30"/>
+      <c r="AJ28" s="54"/>
+      <c r="AK28" s="50"/>
       <c r="AL28" s="30"/>
       <c r="AM28" s="30"/>
-      <c r="AN28" s="32"/>
+      <c r="AN28" s="30"/>
       <c r="AO28" s="32"/>
       <c r="AP28" s="32"/>
       <c r="AQ28" s="32"/>
-      <c r="AR28" s="30"/>
+      <c r="AR28" s="32"/>
       <c r="AS28" s="30"/>
-      <c r="AT28" s="25"/>
+      <c r="AT28" s="30"/>
       <c r="AU28" s="25"/>
-      <c r="AV28" s="26"/>
+      <c r="AV28" s="25"/>
       <c r="AW28" s="26"/>
       <c r="AX28" s="26"/>
       <c r="AY28" s="26"/>
-    </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ28" s="26"/>
+    </row>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="J29" s="12"/>
-      <c r="AD29" s="27"/>
-      <c r="AE29" s="28"/>
+      <c r="B29" s="4"/>
+      <c r="K29" s="12"/>
+      <c r="AE29" s="27"/>
       <c r="AF29" s="28"/>
-      <c r="AG29" s="85"/>
-      <c r="AH29" s="54"/>
+      <c r="AG29" s="28"/>
+      <c r="AH29" s="84"/>
       <c r="AI29" s="54"/>
-      <c r="AJ29" s="50"/>
-      <c r="AK29" s="30"/>
+      <c r="AJ29" s="54"/>
+      <c r="AK29" s="50"/>
       <c r="AL29" s="30"/>
       <c r="AM29" s="30"/>
-      <c r="AN29" s="32"/>
+      <c r="AN29" s="30"/>
       <c r="AO29" s="32"/>
       <c r="AP29" s="32"/>
       <c r="AQ29" s="32"/>
-      <c r="AR29" s="30"/>
+      <c r="AR29" s="32"/>
       <c r="AS29" s="30"/>
       <c r="AT29" s="30"/>
-    </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AU29" s="30"/>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="J31" s="12"/>
-      <c r="AD31" s="27"/>
-      <c r="AE31" s="28"/>
+      <c r="B30" s="4"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="K31" s="12"/>
+      <c r="AE31" s="27"/>
       <c r="AF31" s="28"/>
-      <c r="AG31" s="85"/>
-      <c r="AH31" s="54"/>
+      <c r="AG31" s="28"/>
+      <c r="AH31" s="84"/>
       <c r="AI31" s="54"/>
-      <c r="AJ31" s="50"/>
-      <c r="AK31" s="30"/>
+      <c r="AJ31" s="54"/>
+      <c r="AK31" s="50"/>
       <c r="AL31" s="30"/>
       <c r="AM31" s="30"/>
-      <c r="AN31" s="32"/>
+      <c r="AN31" s="30"/>
       <c r="AO31" s="32"/>
       <c r="AP31" s="32"/>
       <c r="AQ31" s="32"/>
-      <c r="AR31" s="30"/>
+      <c r="AR31" s="32"/>
       <c r="AS31" s="30"/>
       <c r="AT31" s="30"/>
-    </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AU31" s="30"/>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="J32" s="12"/>
-      <c r="AE32" s="28"/>
+      <c r="B32" s="4"/>
+      <c r="K32" s="12"/>
       <c r="AF32" s="28"/>
-      <c r="AG32" s="85"/>
-      <c r="AH32" s="54"/>
+      <c r="AG32" s="28"/>
+      <c r="AH32" s="84"/>
       <c r="AI32" s="54"/>
-      <c r="AJ32" s="50"/>
-      <c r="AK32" s="30"/>
+      <c r="AJ32" s="54"/>
+      <c r="AK32" s="50"/>
       <c r="AL32" s="30"/>
       <c r="AM32" s="30"/>
-      <c r="AN32" s="32"/>
+      <c r="AN32" s="30"/>
       <c r="AO32" s="32"/>
       <c r="AP32" s="32"/>
       <c r="AQ32" s="32"/>
-      <c r="AR32" s="30"/>
+      <c r="AR32" s="32"/>
       <c r="AS32" s="30"/>
       <c r="AT32" s="30"/>
       <c r="AU32" s="30"/>
-    </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="J33" s="12"/>
-      <c r="AF33" s="28"/>
-      <c r="AG33" s="85"/>
-      <c r="AH33" s="54"/>
+      <c r="AV32" s="30"/>
+    </row>
+    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="K33" s="12"/>
+      <c r="AG33" s="28"/>
+      <c r="AH33" s="84"/>
       <c r="AI33" s="54"/>
-      <c r="AJ33" s="50"/>
-      <c r="AK33" s="30"/>
+      <c r="AJ33" s="54"/>
+      <c r="AK33" s="50"/>
       <c r="AL33" s="30"/>
       <c r="AM33" s="30"/>
-      <c r="AN33" s="32"/>
+      <c r="AN33" s="30"/>
       <c r="AO33" s="32"/>
       <c r="AP33" s="32"/>
       <c r="AQ33" s="32"/>
-      <c r="AR33" s="30"/>
+      <c r="AR33" s="32"/>
       <c r="AS33" s="30"/>
       <c r="AT33" s="30"/>
       <c r="AU33" s="30"/>
-      <c r="AV33" s="32"/>
-    </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AV33" s="30"/>
+      <c r="AW33" s="32"/>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="J34" s="12"/>
-    </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="J35" s="12"/>
-      <c r="AF35" s="28"/>
-      <c r="AG35" s="85"/>
-      <c r="AH35" s="54"/>
+      <c r="B34" s="2"/>
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="K35" s="12"/>
+      <c r="AG35" s="28"/>
+      <c r="AH35" s="84"/>
       <c r="AI35" s="54"/>
-      <c r="AJ35" s="50"/>
-      <c r="AK35" s="30"/>
+      <c r="AJ35" s="54"/>
+      <c r="AK35" s="50"/>
       <c r="AL35" s="30"/>
       <c r="AM35" s="30"/>
-      <c r="AN35" s="32"/>
+      <c r="AN35" s="30"/>
       <c r="AO35" s="32"/>
       <c r="AP35" s="32"/>
       <c r="AQ35" s="32"/>
-      <c r="AR35" s="30"/>
+      <c r="AR35" s="32"/>
       <c r="AS35" s="30"/>
       <c r="AT35" s="30"/>
       <c r="AU35" s="30"/>
-      <c r="AV35" s="32"/>
-    </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AV35" s="30"/>
+      <c r="AW35" s="32"/>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="J36" s="12"/>
-      <c r="AG36" s="85"/>
-      <c r="AH36" s="54"/>
+      <c r="B36" s="2"/>
+      <c r="K36" s="12"/>
+      <c r="AH36" s="84"/>
       <c r="AI36" s="54"/>
-      <c r="AJ36" s="50"/>
-      <c r="AK36" s="30"/>
+      <c r="AJ36" s="54"/>
+      <c r="AK36" s="50"/>
       <c r="AL36" s="30"/>
       <c r="AM36" s="30"/>
-      <c r="AN36" s="32"/>
+      <c r="AN36" s="30"/>
       <c r="AO36" s="32"/>
       <c r="AP36" s="32"/>
       <c r="AQ36" s="32"/>
-      <c r="AR36" s="30"/>
+      <c r="AR36" s="32"/>
       <c r="AS36" s="30"/>
       <c r="AT36" s="30"/>
       <c r="AU36" s="30"/>
-      <c r="AV36" s="32"/>
+      <c r="AV36" s="30"/>
       <c r="AW36" s="32"/>
-    </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="B37" s="40"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="42"/>
+      <c r="AX36" s="32"/>
+    </row>
+    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="C37" s="40"/>
+      <c r="D37" s="41"/>
       <c r="E37" s="42"/>
       <c r="F37" s="42"/>
-      <c r="G37" s="43"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="43"/>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
-      <c r="K37" s="42"/>
+      <c r="K37" s="43"/>
       <c r="L37" s="42"/>
       <c r="M37" s="42"/>
       <c r="N37" s="42"/>
-      <c r="O37" s="43"/>
+      <c r="O37" s="42"/>
       <c r="P37" s="43"/>
       <c r="Q37" s="43"/>
-      <c r="R37" s="44"/>
-      <c r="S37" s="42"/>
+      <c r="R37" s="43"/>
+      <c r="S37" s="44"/>
       <c r="T37" s="42"/>
       <c r="U37" s="42"/>
       <c r="V37" s="42"/>
-      <c r="W37" s="43"/>
+      <c r="W37" s="42"/>
       <c r="X37" s="43"/>
       <c r="Y37" s="43"/>
       <c r="Z37" s="43"/>
-      <c r="AA37" s="42"/>
+      <c r="AA37" s="43"/>
       <c r="AB37" s="42"/>
       <c r="AC37" s="42"/>
       <c r="AD37" s="42"/>
-      <c r="AE37" s="43"/>
+      <c r="AE37" s="42"/>
       <c r="AF37" s="43"/>
-      <c r="AG37" s="87"/>
-      <c r="AH37" s="54"/>
+      <c r="AG37" s="43"/>
+      <c r="AH37" s="86"/>
       <c r="AI37" s="54"/>
-      <c r="AJ37" s="50"/>
-      <c r="AK37" s="30"/>
+      <c r="AJ37" s="54"/>
+      <c r="AK37" s="50"/>
       <c r="AL37" s="30"/>
       <c r="AM37" s="30"/>
-      <c r="AN37" s="32"/>
+      <c r="AN37" s="30"/>
       <c r="AO37" s="32"/>
       <c r="AP37" s="32"/>
       <c r="AQ37" s="32"/>
-      <c r="AR37" s="30"/>
+      <c r="AR37" s="32"/>
       <c r="AS37" s="30"/>
       <c r="AT37" s="30"/>
       <c r="AU37" s="30"/>
-      <c r="AV37" s="32"/>
+      <c r="AV37" s="30"/>
       <c r="AW37" s="32"/>
       <c r="AX37" s="32"/>
-    </row>
-    <row r="38" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AY37" s="32"/>
+    </row>
+    <row r="38" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
-      <c r="B38" s="68"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="27"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="69"/>
       <c r="E38" s="27"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="48"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="47"/>
       <c r="H38" s="48"/>
       <c r="I38" s="48"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="27"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="28"/>
       <c r="L38" s="27"/>
       <c r="M38" s="27"/>
-      <c r="N38" s="47"/>
-      <c r="O38" s="48"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="47"/>
       <c r="P38" s="48"/>
       <c r="Q38" s="48"/>
-      <c r="R38" s="63"/>
-      <c r="S38" s="27"/>
+      <c r="R38" s="48"/>
+      <c r="S38" s="63"/>
       <c r="T38" s="27"/>
       <c r="U38" s="27"/>
-      <c r="V38" s="47"/>
-      <c r="W38" s="48"/>
+      <c r="V38" s="27"/>
+      <c r="W38" s="47"/>
       <c r="X38" s="48"/>
       <c r="Y38" s="48"/>
-      <c r="Z38" s="28"/>
-      <c r="AA38" s="27"/>
+      <c r="Z38" s="48"/>
+      <c r="AA38" s="28"/>
       <c r="AB38" s="27"/>
       <c r="AC38" s="27"/>
-      <c r="AD38" s="47"/>
-      <c r="AE38" s="48"/>
+      <c r="AD38" s="27"/>
+      <c r="AE38" s="47"/>
       <c r="AF38" s="48"/>
-      <c r="AG38" s="85"/>
-      <c r="AH38" s="54"/>
+      <c r="AG38" s="48"/>
+      <c r="AH38" s="84"/>
       <c r="AI38" s="54"/>
-      <c r="AJ38" s="50"/>
-      <c r="AK38" s="30"/>
+      <c r="AJ38" s="54"/>
+      <c r="AK38" s="50"/>
       <c r="AL38" s="30"/>
       <c r="AM38" s="30"/>
-      <c r="AN38" s="32"/>
+      <c r="AN38" s="30"/>
       <c r="AO38" s="32"/>
       <c r="AP38" s="32"/>
       <c r="AQ38" s="32"/>
-      <c r="AR38" s="30"/>
+      <c r="AR38" s="32"/>
       <c r="AS38" s="30"/>
       <c r="AT38" s="30"/>
       <c r="AU38" s="30"/>
-      <c r="AV38" s="32"/>
+      <c r="AV38" s="30"/>
       <c r="AW38" s="32"/>
       <c r="AX38" s="32"/>
       <c r="AY38" s="32"/>
-    </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="J39" s="12"/>
-    </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ38" s="32"/>
+    </row>
+    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="K39" s="12"/>
+    </row>
+    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="J40" s="12"/>
-    </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="J42" s="12"/>
+      <c r="B40" s="2"/>
+      <c r="K40" s="12"/>
+    </row>
+    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="K41" s="12"/>
+    </row>
+    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="K42" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>